<commit_message>
Menu finalizado e testado
Inserir lista
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,17 +507,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['1', 't6959989']</t>
+          <t>['1', 't6959989', 't8890634']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['g2422223', 'g0330150']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[7.14]</t>
+          <t>[7.14, 5.69]</t>
         </is>
       </c>
     </row>
@@ -549,12 +549,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['1']</t>
+          <t>['1', 't8890634']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['g0330150']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -634,6 +634,82 @@
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ra9392101</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ra9392101</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>juao</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>aa@aa.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ra8095505</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ra8095505</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>daniel</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>bb@bb.com</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -646,7 +722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,7 +780,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[{'id': '1', 'nome': 'C1', 'data_de_inicio': '12', 'data_de_fim': '21', 'peso_da_nota': '3'}, {'id': '2', 'nome': 'C2', 'data_de_inicio': '23', 'data_de_fim': '32', 'peso_da_nota': '4'}, {'id': 'c9878959', 'nome': 'C3', 'data_de_inicio': '12/12/2024', 'data_de_fim': '13/12/2024', 'peso_da_nota': '6'}, {'id': 'c4088151', 'nome': 'aba', 'data_de_inicio': '02/10/2024', 'data_de_fim': '01/11/2024', 'peso_da_nota': '5'}, {'id': 'c4238120', 'nome': 'c4', 'data_de_inicio': '27/11/2023', 'data_de_fim': '28/11/2023', 'peso_da_nota': '6'}, {'id': 'c1773595', 'nome': 'aaaaa', 'data_de_inicio': '27/11/2023', 'data_de_fim': '27/12/2023', 'peso_da_nota': '7'}]</t>
+          <t>[{'id': '1', 'nome': 'C1', 'data_de_inicio': '12', 'data_de_fim': '21', 'peso_da_nota': '3'}, {'id': '2', 'nome': 'C2', 'data_de_inicio': '23', 'data_de_fim': '32', 'peso_da_nota': '4'}, {'id': 'c9878959', 'nome': 'C3', 'data_de_inicio': '12/12/2024', 'data_de_fim': '13/12/2024', 'peso_da_nota': '6'}, {'id': 'c4088151', 'nome': 'aba', 'data_de_inicio': '02/10/2024', 'data_de_fim': '01/11/2024', 'peso_da_nota': '5'}, {'id': 'c4238120', 'nome': 'c4', 'data_de_inicio': '27/11/2023', 'data_de_fim': '28/11/2023', 'peso_da_nota': '6'}, {'id': 'c1773595', 'nome': 'aaaaa', 'data_de_inicio': '27/11/2023', 'data_de_fim': '27/12/2023', 'peso_da_nota': '7'}, {'id': 'c5717717', 'nome': '3', 'data_de_inicio': '12/12/2023', 'data_de_fim': '12/12/2023', 'peso_da_nota': '6'}, {'id': 'c6884323', 'nome': 'c9878959', 'data_de_inicio': '28/11/2023', 'data_de_fim': '29/11/2023', 'peso_da_nota': '6'}, {'id': 'c5390957', 'nome': 'aaaaaaaa', 'data_de_inicio': '29/11/2023', 'data_de_fim': '30/11/2023', 'peso_da_nota': '7'}]</t>
         </is>
       </c>
     </row>
@@ -803,6 +879,29 @@
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>t8890634</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>t8890634</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>os batutinhas</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>31/01/2024</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -815,7 +914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,30 +1149,126 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>c5717717</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>c5717717</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12/12/2023</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12/12/2023</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c6884323</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>c6884323</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>c9878959</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>28/11/2023</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>29/11/2023</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>c5390957</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>c5390957</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>aaaaaaaa</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>29/11/2023</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>30/11/2023</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>c6577440</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>c6577440</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Python</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>12/12/2023</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>01/01/2024</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1090,7 +1285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1137,6 +1332,94 @@
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>['1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>g2391477</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>g2391477</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>hobbit's house</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['1', '1', '1', '1', '1', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>daaaa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['1', '1', '1', '1', '1', '1', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>g2422223</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>g2422223</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>g0330150</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>g0330150</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>faa</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>['1', '2']</t>
         </is>
@@ -1153,7 +1436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1210,7 +1493,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -1236,6 +1519,31 @@
       </c>
       <c r="E3" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ID3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>c1773595</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pos teste e listagem
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +517,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[7.14, 5.69]</t>
+          <t>[7.14, 5.69, 5.69]</t>
         </is>
       </c>
     </row>
@@ -710,6 +710,82 @@
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ra054</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ra054</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>daniel</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>da@da.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ra432</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ra432</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>junn</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>dani@dan.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -722,7 +798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,7 +856,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[{'id': '1', 'nome': 'C1', 'data_de_inicio': '12', 'data_de_fim': '21', 'peso_da_nota': '3'}, {'id': '2', 'nome': 'C2', 'data_de_inicio': '23', 'data_de_fim': '32', 'peso_da_nota': '4'}, {'id': 'c9878959', 'nome': 'C3', 'data_de_inicio': '12/12/2024', 'data_de_fim': '13/12/2024', 'peso_da_nota': '6'}, {'id': 'c4088151', 'nome': 'aba', 'data_de_inicio': '02/10/2024', 'data_de_fim': '01/11/2024', 'peso_da_nota': '5'}, {'id': 'c4238120', 'nome': 'c4', 'data_de_inicio': '27/11/2023', 'data_de_fim': '28/11/2023', 'peso_da_nota': '6'}, {'id': 'c1773595', 'nome': 'aaaaa', 'data_de_inicio': '27/11/2023', 'data_de_fim': '27/12/2023', 'peso_da_nota': '7'}, {'id': 'c5717717', 'nome': '3', 'data_de_inicio': '12/12/2023', 'data_de_fim': '12/12/2023', 'peso_da_nota': '6'}, {'id': 'c6884323', 'nome': 'c9878959', 'data_de_inicio': '28/11/2023', 'data_de_fim': '29/11/2023', 'peso_da_nota': '6'}, {'id': 'c5390957', 'nome': 'aaaaaaaa', 'data_de_inicio': '29/11/2023', 'data_de_fim': '30/11/2023', 'peso_da_nota': '7'}]</t>
+          <t>[{'id': '1', 'nome': 'C1', 'data_de_inicio': '12', 'data_de_fim': '21', 'peso_da_nota': '3'}, {'id': '2', 'nome': 'C2', 'data_de_inicio': '23', 'data_de_fim': '32', 'peso_da_nota': '4'}, {'id': 'c9878959', 'nome': 'C3', 'data_de_inicio': '12/12/2024', 'data_de_fim': '13/12/2024', 'peso_da_nota': '6'}, {'id': 'c4088151', 'nome': 'aba', 'data_de_inicio': '02/10/2024', 'data_de_fim': '01/11/2024', 'peso_da_nota': '5'}, {'id': 'c4238120', 'nome': 'c4', 'data_de_inicio': '27/11/2023', 'data_de_fim': '28/11/2023', 'peso_da_nota': '6'}, {'id': 'c1773595', 'nome': 'aaaaa', 'data_de_inicio': '27/11/2023', 'data_de_fim': '27/12/2023', 'peso_da_nota': '7'}, {'id': 'c5717717', 'nome': '3', 'data_de_inicio': '12/12/2023', 'data_de_fim': '12/12/2023', 'peso_da_nota': '6'}, {'id': 'c6884323', 'nome': 'c9878959', 'data_de_inicio': '28/11/2023', 'data_de_fim': '29/11/2023', 'peso_da_nota': '6'}, {'id': 'c5390957', 'nome': 'aaaaaaaa', 'data_de_inicio': '29/11/2023', 'data_de_fim': '30/11/2023', 'peso_da_nota': '7'}, {'id': 'C882', 'nome': 'nadalete ', 'data_de_inicio': '27/11/2023', 'data_de_fim': '27/12/2023', 'peso_da_nota': '5'}]</t>
         </is>
       </c>
     </row>
@@ -902,6 +978,56 @@
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>t3093321</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>t3093321</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>app</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>20/12/2023</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>t5300480</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>t5300480</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>12/12/2023</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[{'id': 'C039', 'nome': 'java', 'data_de_inicio': '12/12/2024', 'data_de_fim': '13/12/2024', 'peso_da_nota': '6'}]</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -914,7 +1040,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1245,32 +1371,96 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>C882</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C882</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nadalete </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>27/11/2023</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>27/12/2023</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>c6577440</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>c6577440</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Python</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>12/12/2023</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>01/01/2024</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C039</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C039</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12/12/2024</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -1285,7 +1475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1422,6 +1612,28 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>['1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>G435</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>G435</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>['ra054']</t>
         </is>
       </c>
     </row>

</xml_diff>